<commit_message>
new config 5 Digit
</commit_message>
<xml_diff>
--- a/tables/MB18_thresholds_5D.xlsx
+++ b/tables/MB18_thresholds_5D.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francescopiscitelli/Documents/PYTHON/MBUTY/tables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francescopiscitelli/Documents/MATLAB/004_CAEN_visualizationDPPtraces/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD43DAFC-F347-8B48-A017-F091CACF5906}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A165D018-1D3E-CC4E-BF9F-6140FE5DD46F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14560" yWindow="460" windowWidth="13740" windowHeight="16340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -368,7 +368,7 @@
   <dimension ref="A1:E65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -384,7 +384,7 @@
         <v>33</v>
       </c>
       <c r="C1">
-        <v>124</v>
+        <v>142</v>
       </c>
       <c r="D1">
         <v>143</v>
@@ -395,529 +395,529 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
+        <v>12380.95238095238</v>
+      </c>
+      <c r="B2">
         <v>5000</v>
-      </c>
-      <c r="B2">
-        <v>12380.95238095238</v>
       </c>
       <c r="C2">
         <v>5000</v>
       </c>
       <c r="D2">
-        <v>5000</v>
+        <v>7000</v>
       </c>
       <c r="E2">
-        <v>7000</v>
+        <v>10500</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>5000</v>
+        <v>16190.476190476189</v>
       </c>
       <c r="B3">
-        <v>16190.476190476189</v>
+        <v>14000</v>
       </c>
       <c r="C3">
-        <v>14000</v>
+        <v>15000</v>
       </c>
       <c r="D3">
-        <v>15000</v>
+        <v>7000</v>
       </c>
       <c r="E3">
-        <v>7000</v>
+        <v>18500</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>5000</v>
+        <v>14761.904761904761</v>
       </c>
       <c r="B4">
-        <v>14761.904761904761</v>
+        <v>13000</v>
       </c>
       <c r="C4">
-        <v>13000</v>
+        <v>14000</v>
       </c>
       <c r="D4">
-        <v>14000</v>
+        <v>7000</v>
       </c>
       <c r="E4">
-        <v>7000</v>
+        <v>19500</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>5000</v>
+        <v>14761.904761904761</v>
       </c>
       <c r="B5">
-        <v>14761.904761904761</v>
+        <v>14000</v>
       </c>
       <c r="C5">
-        <v>14000</v>
+        <v>15000</v>
       </c>
       <c r="D5">
-        <v>15000</v>
+        <v>7000</v>
       </c>
       <c r="E5">
-        <v>7000</v>
+        <v>19500</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>5000</v>
+        <v>17142.857142857141</v>
       </c>
       <c r="B6">
-        <v>17142.857142857141</v>
+        <v>19000</v>
       </c>
       <c r="C6">
-        <v>19000</v>
+        <v>16000</v>
       </c>
       <c r="D6">
-        <v>16000</v>
+        <v>7000</v>
       </c>
       <c r="E6">
-        <v>7000</v>
+        <v>21500</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>5000</v>
+        <v>13333.333333333332</v>
       </c>
       <c r="B7">
-        <v>13333.333333333332</v>
+        <v>12000</v>
       </c>
       <c r="C7">
-        <v>12000</v>
+        <v>10000</v>
       </c>
       <c r="D7">
-        <v>10000</v>
+        <v>7000</v>
       </c>
       <c r="E7">
-        <v>7000</v>
+        <v>15000</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>10500</v>
+        <v>15238.095238095237</v>
       </c>
       <c r="B8">
-        <v>15238.095238095237</v>
+        <v>17073.170731707316</v>
       </c>
       <c r="C8">
-        <v>17073.170731707316</v>
+        <v>15000</v>
       </c>
       <c r="D8">
-        <v>15000</v>
+        <v>12195.121951219511</v>
       </c>
       <c r="E8">
-        <v>12195.121951219511</v>
+        <v>19744.483159117302</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>9000</v>
+        <v>15873.015873015869</v>
       </c>
       <c r="B9">
-        <v>15873.015873015869</v>
+        <v>16666.666666666664</v>
       </c>
       <c r="C9">
-        <v>16666.666666666664</v>
+        <v>17000</v>
       </c>
       <c r="D9">
-        <v>17000</v>
+        <v>11904.761904761903</v>
       </c>
       <c r="E9">
-        <v>11904.761904761903</v>
+        <v>19274.376417233558</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>12000</v>
+        <v>15503.875968992246</v>
       </c>
       <c r="B10">
-        <v>15503.875968992246</v>
+        <v>16279.069767441859</v>
       </c>
       <c r="C10">
         <v>16279.069767441859</v>
       </c>
       <c r="D10">
-        <v>16279.069767441859</v>
+        <v>11627.906976744185</v>
       </c>
       <c r="E10">
-        <v>11627.906976744185</v>
+        <v>18826.13510520487</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>5000</v>
+        <v>15151.515151515152</v>
       </c>
       <c r="B11">
-        <v>15151.515151515152</v>
+        <v>15909.09090909091</v>
       </c>
       <c r="C11">
         <v>15909.09090909091</v>
       </c>
       <c r="D11">
-        <v>15909.09090909091</v>
+        <v>11363.636363636364</v>
       </c>
       <c r="E11">
-        <v>11363.636363636364</v>
+        <v>18398.268398268399</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>12500</v>
+        <v>14814.814814814814</v>
       </c>
       <c r="B12">
-        <v>14814.814814814814</v>
+        <v>15000</v>
       </c>
       <c r="C12">
-        <v>15000</v>
+        <v>15555.555555555555</v>
       </c>
       <c r="D12">
-        <v>15555.555555555555</v>
+        <v>11111.111111111111</v>
       </c>
       <c r="E12">
-        <v>11111.111111111111</v>
+        <v>18888.888888888887</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>13000</v>
+        <v>15942.028985507248</v>
       </c>
       <c r="B13">
-        <v>15942.028985507248</v>
+        <v>15217.391304347826</v>
       </c>
       <c r="C13">
         <v>15217.391304347826</v>
       </c>
       <c r="D13">
-        <v>15217.391304347826</v>
+        <v>12000</v>
       </c>
       <c r="E13">
-        <v>12000</v>
+        <v>18478.260869565216</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>12500</v>
+        <v>15602.836879432623</v>
       </c>
       <c r="B14">
-        <v>15602.836879432623</v>
+        <v>14893.617021276596</v>
       </c>
       <c r="C14">
         <v>14893.617021276596</v>
       </c>
       <c r="D14">
-        <v>14893.617021276596</v>
+        <v>14000</v>
       </c>
       <c r="E14">
-        <v>14000</v>
+        <v>18500</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>8000</v>
+        <v>15238.095238095237</v>
       </c>
       <c r="B15">
-        <v>15238.095238095237</v>
+        <v>14583.333333333332</v>
       </c>
       <c r="C15">
-        <v>14583.333333333332</v>
+        <v>15500</v>
       </c>
       <c r="D15">
-        <v>15500</v>
+        <v>14000</v>
       </c>
       <c r="E15">
-        <v>14000</v>
+        <v>18500</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>9142.8571428571431</v>
+        <v>12571.428571428572</v>
       </c>
       <c r="B16">
-        <v>12571.428571428572</v>
+        <v>14285.714285714286</v>
       </c>
       <c r="C16">
         <v>14285.714285714286</v>
       </c>
       <c r="D16">
-        <v>14285.714285714286</v>
+        <v>12000</v>
       </c>
       <c r="E16">
-        <v>12000</v>
+        <v>16500</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>10500</v>
+        <v>14666.666666666668</v>
       </c>
       <c r="B17">
-        <v>14666.666666666668</v>
+        <v>15000</v>
       </c>
       <c r="C17">
-        <v>15000</v>
+        <v>13000</v>
       </c>
       <c r="D17">
-        <v>13000</v>
+        <v>12000</v>
       </c>
       <c r="E17">
-        <v>12000</v>
+        <v>18000</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>8000</v>
+        <v>14379.084967320263</v>
       </c>
       <c r="B18">
-        <v>14379.084967320263</v>
+        <v>13725.490196078432</v>
       </c>
       <c r="C18">
         <v>13725.490196078432</v>
       </c>
       <c r="D18">
-        <v>13725.490196078432</v>
+        <v>12000</v>
       </c>
       <c r="E18">
-        <v>12000</v>
+        <v>17000</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>8000</v>
+        <v>12820.51282051282</v>
       </c>
       <c r="B19">
-        <v>12820.51282051282</v>
+        <v>13461.538461538461</v>
       </c>
       <c r="C19">
         <v>13461.538461538461</v>
       </c>
       <c r="D19">
-        <v>13461.538461538461</v>
+        <v>12000</v>
       </c>
       <c r="E19">
-        <v>12000</v>
+        <v>15000</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>8000</v>
+        <v>12578.616352201256</v>
       </c>
       <c r="B20">
-        <v>12578.616352201256</v>
+        <v>13207.54716981132</v>
       </c>
       <c r="C20">
         <v>13207.54716981132</v>
       </c>
       <c r="D20">
-        <v>13207.54716981132</v>
+        <v>12500</v>
       </c>
       <c r="E20">
-        <v>12500</v>
+        <v>15000</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>8000</v>
+        <v>13580.246913580246</v>
       </c>
       <c r="B21">
-        <v>13580.246913580246</v>
+        <v>14000</v>
       </c>
       <c r="C21">
         <v>14000</v>
       </c>
       <c r="D21">
-        <v>14000</v>
+        <v>12000</v>
       </c>
       <c r="E21">
-        <v>12000</v>
+        <v>15500</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>10000</v>
+        <v>13809.523809523809</v>
       </c>
       <c r="B22">
-        <v>13809.523809523809</v>
+        <v>12727.272727272726</v>
       </c>
       <c r="C22">
         <v>12727.272727272726</v>
       </c>
       <c r="D22">
-        <v>12727.272727272726</v>
+        <v>11000</v>
       </c>
       <c r="E22">
-        <v>11000</v>
+        <v>18500</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>10000</v>
+        <v>13095.238095238095</v>
       </c>
       <c r="B23">
-        <v>13095.238095238095</v>
+        <v>12499.999999999998</v>
       </c>
       <c r="C23">
         <v>12499.999999999998</v>
       </c>
       <c r="D23">
-        <v>12499.999999999998</v>
+        <v>12500</v>
       </c>
       <c r="E23">
-        <v>12500</v>
+        <v>15178.571428571428</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>5000</v>
+        <v>12865.497076023392</v>
       </c>
       <c r="B24">
-        <v>12865.497076023392</v>
+        <v>12280.701754385964</v>
       </c>
       <c r="C24">
         <v>12280.701754385964</v>
       </c>
       <c r="D24">
-        <v>12280.701754385964</v>
+        <v>11000</v>
       </c>
       <c r="E24">
-        <v>11000</v>
+        <v>13000</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>8034.4827586206893</v>
+        <v>12643.67816091954</v>
       </c>
       <c r="B25">
-        <v>12643.67816091954</v>
+        <v>12068.965517241379</v>
       </c>
       <c r="C25">
         <v>12068.965517241379</v>
       </c>
       <c r="D25">
-        <v>12068.965517241379</v>
+        <v>12500</v>
       </c>
       <c r="E25">
-        <v>12500</v>
+        <v>13500</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>6000</v>
+        <v>12429.378531073446</v>
       </c>
       <c r="B26">
-        <v>12429.378531073446</v>
+        <v>11864.406779661016</v>
       </c>
       <c r="C26">
         <v>11864.406779661016</v>
       </c>
       <c r="D26">
-        <v>11864.406779661016</v>
+        <v>12000</v>
       </c>
       <c r="E26">
-        <v>12000</v>
+        <v>14406.779661016948</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>6000</v>
+        <v>13333.333333333332</v>
       </c>
       <c r="B27">
-        <v>13333.333333333332</v>
+        <v>11666.666666666664</v>
       </c>
       <c r="C27">
         <v>11666.666666666664</v>
       </c>
       <c r="D27">
-        <v>11666.666666666664</v>
+        <v>13000</v>
       </c>
       <c r="E27">
-        <v>13000</v>
+        <v>14166.666666666664</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>6000</v>
+        <v>12021.857923497269</v>
       </c>
       <c r="B28">
-        <v>12021.857923497269</v>
+        <v>11475.409836065573</v>
       </c>
       <c r="C28">
         <v>11475.409836065573</v>
       </c>
       <c r="D28">
-        <v>11475.409836065573</v>
+        <v>9000</v>
       </c>
       <c r="E28">
-        <v>9000</v>
+        <v>15000</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>6000</v>
+        <v>11827.956989247312</v>
       </c>
       <c r="B29">
-        <v>11827.956989247312</v>
+        <v>11290.322580645161</v>
       </c>
       <c r="C29">
         <v>11290.322580645161</v>
       </c>
       <c r="D29">
-        <v>11290.322580645161</v>
+        <v>9000</v>
       </c>
       <c r="E29">
-        <v>9000</v>
+        <v>13709.677419354839</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>6000</v>
+        <v>11640.211640211641</v>
       </c>
       <c r="B30">
-        <v>11640.211640211641</v>
+        <v>11111.111111111111</v>
       </c>
       <c r="C30">
         <v>11111.111111111111</v>
       </c>
       <c r="D30">
-        <v>11111.111111111111</v>
+        <v>9000</v>
       </c>
       <c r="E30">
-        <v>9000</v>
+        <v>13492.063492063491</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>6000</v>
+        <v>11458.333333333334</v>
       </c>
       <c r="B31">
-        <v>11458.333333333334</v>
+        <v>10937.5</v>
       </c>
       <c r="C31">
         <v>10937.5</v>
       </c>
       <c r="D31">
-        <v>10937.5</v>
+        <v>9000</v>
       </c>
       <c r="E31">
-        <v>9000</v>
+        <v>13281.25</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>6000</v>
+        <v>11282.051282051283</v>
       </c>
       <c r="B32">
-        <v>11282.051282051283</v>
+        <v>10769.23076923077</v>
       </c>
       <c r="C32">
         <v>10769.23076923077</v>
       </c>
       <c r="D32">
-        <v>10769.23076923077</v>
+        <v>9000</v>
       </c>
       <c r="E32">
-        <v>9000</v>
+        <v>13076.923076923076</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>